<commit_message>
add functions to db
</commit_message>
<xml_diff>
--- a/base.xlsx
+++ b/base.xlsx
@@ -9,39 +9,56 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="stickers" sheetId="1" r:id="rId1"/>
+    <sheet name="users" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Ключевая фраза</t>
   </si>
   <si>
+    <t>file.id</t>
+  </si>
+  <si>
+    <t>Answer</t>
+  </si>
+  <si>
     <t>Привет</t>
   </si>
   <si>
+    <t>CAACAgIAAxkBAAPwYgOYLTqiqDRaosBXwhdlM-YCNGgAAkQSAAKat6FL-O5ub_QpkuUjBA</t>
+  </si>
+  <si>
     <t>Пока</t>
   </si>
   <si>
-    <t>file.id</t>
-  </si>
-  <si>
     <t>CAACAgIAAxkBAAIBBWIDoFuXpZ1fjuFcFjJ3Rnv_QhkpAALREgACq03JSwiCbNDIBAFQIwQ</t>
   </si>
   <si>
-    <t>CAACAgIAAxkBAAPwYgOYLTqiqDRaosBXwhdlM-YCNGgAAkQSAAKat6FL-O5ub_QpkuUjBA</t>
+    <t>До свидания</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Здравствуйте!</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>grade</t>
   </si>
 </sst>
 </file>
@@ -369,44 +386,95 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="24.42578125" customWidth="1"/>
     <col min="2" max="2" width="84.140625" customWidth="1"/>
+    <col min="3" max="3" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
       <c r="B3" s="1" t="s">
-        <v>4</v>
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="4" max="4" width="5.5703125" customWidth="1"/>
+    <col min="5" max="5" width="101.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>